<commit_message>
Tambah hasil scrap dalam format .csv
</commit_message>
<xml_diff>
--- a/PROYEK1-LogBookRegawa.xlsx
+++ b/PROYEK1-LogBookRegawa.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Regawa\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GITREP\Repo-Kel2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>No.</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>13 Maret 2018</t>
+  </si>
+  <si>
+    <t>Mencari web untuk di scrap dan update list web untuk di scrap</t>
+  </si>
+  <si>
+    <t>Scraping data dari web www.pumasera.com</t>
   </si>
 </sst>
 </file>
@@ -134,10 +140,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -421,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,48 +439,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="2"/>
       <c r="D4" t="s">
         <v>20</v>
       </c>
@@ -486,10 +492,10 @@
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="3"/>
       <c r="D5" t="s">
         <v>15</v>
       </c>
@@ -501,10 +507,10 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="3"/>
       <c r="D6" t="s">
         <v>13</v>
       </c>
@@ -516,8 +522,8 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
       <c r="D7" t="s">
         <v>14</v>
       </c>
@@ -529,10 +535,10 @@
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="3"/>
       <c r="D8" t="s">
         <v>13</v>
       </c>
@@ -544,8 +550,8 @@
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
       <c r="D9" t="s">
         <v>16</v>
       </c>
@@ -561,11 +567,25 @@
         <v>22</v>
       </c>
       <c r="C10" s="3"/>
+      <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -579,7 +599,6 @@
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B4:C4"/>
@@ -589,6 +608,7 @@
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:E3"/>
+    <mergeCell ref="B10:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>